<commit_message>
[UPDATE] Radiation impedance calculation - 완료
</commit_message>
<xml_diff>
--- a/1. Arbitrary Array (3,4Array)/Single_FFR_Relative_Error - 최신 HKI 버젼 (integral2 9개 영역).xlsx
+++ b/1. Arbitrary Array (3,4Array)/Single_FFR_Relative_Error - 최신 HKI 버젼 (integral2 9개 영역).xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="35" documentId="6_{3952EC13-6099-488B-A735-225E12CBDEC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{AA317415-FDF4-430D-8AA3-CF2EB0B3F0DB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="17385" xr2:uid="{F809ED7E-B7F2-4D14-9E2F-854BB1B1388F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="17385" activeTab="3" xr2:uid="{F809ED7E-B7F2-4D14-9E2F-854BB1B1388F}"/>
   </bookViews>
   <sheets>
     <sheet name="Z_11" sheetId="1" r:id="rId1"/>
@@ -9032,8 +9032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9057BAD-8FBC-4D49-B900-AD9D698F52D5}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11586,8 +11586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F55ABFB-14F1-408C-BBDD-4655732396A2}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12435,6 +12435,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x0101009AC0F43FD9BF964199581D56114B4C27" ma:contentTypeVersion="11" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="2f94f6736a700a7c3f049d4376f1a16f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="af16c2e8-b6bd-4b6b-b669-c2f78501a31f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="712307dabef5912b330dea80102c9592" ns3:_="">
     <xsd:import namespace="af16c2e8-b6bd-4b6b-b669-c2f78501a31f"/>
@@ -12624,15 +12633,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -12640,6 +12640,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B438D6D-30B2-4C3B-929E-B01871068A79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AB2AC7F-7E56-4991-B160-76050505264E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12657,26 +12665,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B438D6D-30B2-4C3B-929E-B01871068A79}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C131489-7CCA-4670-8B56-C6A51A0F0CAB}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="af16c2e8-b6bd-4b6b-b669-c2f78501a31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="af16c2e8-b6bd-4b6b-b669-c2f78501a31f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>